<commit_message>
write tc 03 and 04,
</commit_message>
<xml_diff>
--- a/src/test/Data/ResultDemo.xlsx
+++ b/src/test/Data/ResultDemo.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="8715" windowWidth="15360" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8715"/>
   </bookViews>
   <sheets>
-    <sheet name="Result" r:id="rId1" sheetId="1"/>
+    <sheet name="Result" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>TC_ID</t>
   </si>
@@ -27,33 +27,11 @@
   <si>
     <t>Note</t>
   </si>
-  <si>
-    <t>TC01</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Nhập nội dung</t>
-  </si>
-  <si>
-    <t>Verify user can login with valid username and password</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,7 +55,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,19 +63,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -114,10 +113,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -315,21 +314,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -346,7 +345,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -398,98 +397,91 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.1171875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="50.75" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.8671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0703125" collapsed="true"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="86.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="18.75" r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>